<commit_message>
modified script for renaming nodes to allow it to run in parallel
</commit_message>
<xml_diff>
--- a/CommunityDetection/communities-stringdb-disease-associations.xlsx
+++ b/CommunityDetection/communities-stringdb-disease-associations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/PycharmProjects/MyGene2Analysis/CommunityDetection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3293CDF-14DD-FF49-AB4C-8B00D1ED5AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34863E5-4646-0949-A726-1ECF0F2CF8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{029E29C8-5BA0-9C45-AA75-518BFA4131FF}"/>
   </bookViews>
@@ -541,7 +541,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>